<commit_message>
Gantt - Diagramm überarbeitet
</commit_message>
<xml_diff>
--- a/Zusätzliches/Diagramme/Gantt Diagramm.xlsx
+++ b/Zusätzliches/Diagramme/Gantt Diagramm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Desktop\Schule\Software\SnakeProjekt\Diagramme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Desktop\Schule\Software\ttth\Zusätzliches\Diagramme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BC19DB-C53E-4DE9-AD15-81ABF122837B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D519FEE5-4AD0-42B3-A807-FDEAF52B8D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F50B8E01-466F-450A-9E3D-73D80AFD844B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Phase</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Marlene</t>
   </si>
 </sst>
 </file>
@@ -518,10 +521,8 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -839,7 +840,7 @@
   <dimension ref="A1:CI13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AY24" sqref="AY24"/>
+      <selection activeCell="AN23" sqref="AN23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,19 +1051,19 @@
       <c r="BN2" s="36">
         <v>44913</v>
       </c>
-      <c r="BO2" s="44">
+      <c r="BO2" s="35">
         <v>44914</v>
       </c>
-      <c r="BP2" s="44">
+      <c r="BP2" s="35">
         <v>44915</v>
       </c>
-      <c r="BQ2" s="44">
+      <c r="BQ2" s="35">
         <v>44916</v>
       </c>
-      <c r="BR2" s="44">
+      <c r="BR2" s="35">
         <v>44917</v>
       </c>
-      <c r="BS2" s="44">
+      <c r="BS2" s="35">
         <v>44918</v>
       </c>
       <c r="BT2" s="36">
@@ -1071,19 +1072,19 @@
       <c r="BU2" s="36">
         <v>44920</v>
       </c>
-      <c r="BV2" s="44">
+      <c r="BV2" s="35">
         <v>44921</v>
       </c>
-      <c r="BW2" s="44">
+      <c r="BW2" s="35">
         <v>44922</v>
       </c>
-      <c r="BX2" s="44">
+      <c r="BX2" s="35">
         <v>44923</v>
       </c>
-      <c r="BY2" s="44">
+      <c r="BY2" s="35">
         <v>44924</v>
       </c>
-      <c r="BZ2" s="44">
+      <c r="BZ2" s="35">
         <v>44925</v>
       </c>
       <c r="CA2" s="36">
@@ -1092,19 +1093,19 @@
       <c r="CB2" s="36">
         <v>44927</v>
       </c>
-      <c r="CC2" s="44">
+      <c r="CC2" s="35">
         <v>44928</v>
       </c>
-      <c r="CD2" s="44">
+      <c r="CD2" s="35">
         <v>44929</v>
       </c>
-      <c r="CE2" s="44">
+      <c r="CE2" s="35">
         <v>44930</v>
       </c>
-      <c r="CF2" s="44">
+      <c r="CF2" s="35">
         <v>44931</v>
       </c>
-      <c r="CG2" s="44">
+      <c r="CG2" s="35">
         <v>44932</v>
       </c>
       <c r="CH2" s="36">
@@ -1199,7 +1200,7 @@
       <c r="BZ3" s="6"/>
       <c r="CA3" s="6"/>
       <c r="CB3" s="6"/>
-      <c r="CC3" s="6"/>
+      <c r="CC3" s="37"/>
       <c r="CD3" s="6"/>
       <c r="CE3" s="6"/>
       <c r="CF3" s="6"/>
@@ -1294,7 +1295,7 @@
       <c r="BZ4" s="2"/>
       <c r="CA4" s="2"/>
       <c r="CB4" s="2"/>
-      <c r="CC4" s="2"/>
+      <c r="CC4" s="37"/>
       <c r="CD4" s="2"/>
       <c r="CE4" s="2"/>
       <c r="CF4" s="2"/>
@@ -1389,7 +1390,7 @@
       <c r="BZ5" s="6"/>
       <c r="CA5" s="6"/>
       <c r="CB5" s="6"/>
-      <c r="CC5" s="6"/>
+      <c r="CC5" s="37"/>
       <c r="CD5" s="6"/>
       <c r="CE5" s="6"/>
       <c r="CF5" s="6"/>
@@ -1405,7 +1406,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="2"/>
@@ -1484,7 +1485,7 @@
       <c r="BZ6" s="2"/>
       <c r="CA6" s="2"/>
       <c r="CB6" s="2"/>
-      <c r="CC6" s="2"/>
+      <c r="CC6" s="37"/>
       <c r="CD6" s="2"/>
       <c r="CE6" s="2"/>
       <c r="CF6" s="2"/>
@@ -1579,7 +1580,7 @@
       <c r="BZ7" s="6"/>
       <c r="CA7" s="6"/>
       <c r="CB7" s="6"/>
-      <c r="CC7" s="6"/>
+      <c r="CC7" s="37"/>
       <c r="CD7" s="6"/>
       <c r="CE7" s="6"/>
       <c r="CF7" s="6"/>
@@ -1674,7 +1675,7 @@
       <c r="BZ8" s="2"/>
       <c r="CA8" s="2"/>
       <c r="CB8" s="2"/>
-      <c r="CC8" s="2"/>
+      <c r="CC8" s="37"/>
       <c r="CD8" s="2"/>
       <c r="CE8" s="2"/>
       <c r="CF8" s="2"/>
@@ -1690,7 +1691,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="6"/>
@@ -1769,7 +1770,7 @@
       <c r="BZ9" s="6"/>
       <c r="CA9" s="6"/>
       <c r="CB9" s="6"/>
-      <c r="CC9" s="6"/>
+      <c r="CC9" s="37"/>
       <c r="CD9" s="6"/>
       <c r="CE9" s="6"/>
       <c r="CF9" s="6"/>
@@ -1864,7 +1865,7 @@
       <c r="BZ10" s="2"/>
       <c r="CA10" s="2"/>
       <c r="CB10" s="2"/>
-      <c r="CC10" s="2"/>
+      <c r="CC10" s="37"/>
       <c r="CD10" s="2"/>
       <c r="CE10" s="2"/>
       <c r="CF10" s="2"/>
@@ -1879,7 +1880,9 @@
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="29"/>
+      <c r="C11" s="29" t="s">
+        <v>25</v>
+      </c>
       <c r="D11" s="10"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -1957,7 +1960,7 @@
       <c r="BZ11" s="38"/>
       <c r="CA11" s="38"/>
       <c r="CB11" s="37"/>
-      <c r="CC11" s="6"/>
+      <c r="CC11" s="37"/>
       <c r="CD11" s="6"/>
       <c r="CE11" s="6"/>
       <c r="CF11" s="6"/>
@@ -2051,7 +2054,7 @@
       <c r="BZ12" s="2"/>
       <c r="CA12" s="2"/>
       <c r="CB12" s="2"/>
-      <c r="CC12" s="2"/>
+      <c r="CC12" s="37"/>
       <c r="CD12" s="2"/>
       <c r="CE12" s="2"/>
       <c r="CF12" s="2"/>
@@ -2066,7 +2069,9 @@
       <c r="B13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="31"/>
+      <c r="C13" s="31" t="s">
+        <v>25</v>
+      </c>
       <c r="D13" s="14"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
@@ -2118,36 +2123,36 @@
       <c r="AZ13" s="19"/>
       <c r="BA13" s="19"/>
       <c r="BB13" s="19"/>
-      <c r="BC13" s="45"/>
-      <c r="BD13" s="45"/>
-      <c r="BE13" s="45"/>
-      <c r="BF13" s="45"/>
-      <c r="BG13" s="45"/>
-      <c r="BH13" s="45"/>
-      <c r="BI13" s="45"/>
-      <c r="BJ13" s="45"/>
-      <c r="BK13" s="45"/>
-      <c r="BL13" s="45"/>
-      <c r="BM13" s="45"/>
-      <c r="BN13" s="45"/>
-      <c r="BO13" s="45"/>
-      <c r="BP13" s="45"/>
-      <c r="BQ13" s="45"/>
-      <c r="BR13" s="45"/>
-      <c r="BS13" s="45"/>
-      <c r="BT13" s="45"/>
-      <c r="BU13" s="45"/>
-      <c r="BV13" s="45"/>
-      <c r="BW13" s="45"/>
-      <c r="BX13" s="45"/>
-      <c r="BY13" s="45"/>
-      <c r="BZ13" s="45"/>
-      <c r="CA13" s="45"/>
+      <c r="BC13" s="19"/>
+      <c r="BD13" s="19"/>
+      <c r="BE13" s="19"/>
+      <c r="BF13" s="19"/>
+      <c r="BG13" s="19"/>
+      <c r="BH13" s="19"/>
+      <c r="BI13" s="19"/>
+      <c r="BJ13" s="19"/>
+      <c r="BK13" s="19"/>
+      <c r="BL13" s="19"/>
+      <c r="BM13" s="19"/>
+      <c r="BN13" s="19"/>
+      <c r="BO13" s="19"/>
+      <c r="BP13" s="19"/>
+      <c r="BQ13" s="19"/>
+      <c r="BR13" s="19"/>
+      <c r="BS13" s="19"/>
+      <c r="BT13" s="19"/>
+      <c r="BU13" s="19"/>
+      <c r="BV13" s="19"/>
+      <c r="BW13" s="19"/>
+      <c r="BX13" s="19"/>
+      <c r="BY13" s="19"/>
+      <c r="BZ13" s="19"/>
+      <c r="CA13" s="19"/>
       <c r="CB13" s="45"/>
-      <c r="CC13" s="45"/>
-      <c r="CD13" s="45"/>
-      <c r="CE13" s="45"/>
-      <c r="CF13" s="45"/>
+      <c r="CC13" s="44"/>
+      <c r="CD13" s="19"/>
+      <c r="CE13" s="19"/>
+      <c r="CF13" s="19"/>
       <c r="CG13" s="19"/>
       <c r="CH13" s="19"/>
       <c r="CI13" s="15"/>

</xml_diff>